<commit_message>
update late plus schedule
</commit_message>
<xml_diff>
--- a/articles/course_docs/cog_2025.xlsx
+++ b/articles/course_docs/cog_2025.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10119"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10209"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/a.kumar/Documents/cognition/articles/course_docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BF4EA82-4C66-344F-AEA1-6BB419897D29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C8327C9-AA16-8A4D-A299-8204B65CC9C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17200" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="105">
   <si>
     <t>Week</t>
   </si>
@@ -171,21 +171,9 @@
     <t>W1 continued…</t>
   </si>
   <si>
-    <t>&lt;b&gt;&lt;span style="color:#8304BA"&gt; Quiz 1 due&lt;/span&gt;&lt;/b&gt;</t>
-  </si>
-  <si>
     <t>W2 continued…</t>
   </si>
   <si>
-    <t>&lt;b&gt;&lt;span style="color:#8304BA"&gt; Quiz 2 due&lt;/span&gt;&lt;/b&gt;</t>
-  </si>
-  <si>
-    <t>&lt;b&gt;&lt;span style="color:#8304BA"&gt; Quiz 3 due&lt;/span&gt;&lt;/b&gt;</t>
-  </si>
-  <si>
-    <t>&lt;b&gt;&lt;span style="color:#8304BA"&gt; Quiz 4 due&lt;/span&gt;&lt;/b&gt;</t>
-  </si>
-  <si>
     <t>&lt;b&gt;&lt;span style="color:#DB5C41"&gt; Final Exam &lt;/span&gt;&lt;/b&gt;</t>
   </si>
   <si>
@@ -195,24 +183,6 @@
     <t>&lt;b&gt;&lt;span style="color:#DB5C41"&gt; Midterm Exam &lt;/span&gt;&lt;/b&gt;</t>
   </si>
   <si>
-    <t>&lt;b&gt;&lt;span style="color:#8304BA"&gt; Quiz 5 due&lt;/span&gt;&lt;/b&gt;</t>
-  </si>
-  <si>
-    <t>&lt;b&gt;&lt;span style="color:#8304BA"&gt; Quiz 6 due&lt;/span&gt;&lt;/b&gt;</t>
-  </si>
-  <si>
-    <t>&lt;b&gt;&lt;span style="color:#8304BA"&gt; Quiz 7 due&lt;/span&gt;&lt;/b&gt;</t>
-  </si>
-  <si>
-    <t>&lt;b&gt;&lt;span style="color:#8304BA"&gt; Quiz 8 due&lt;/span&gt;&lt;/b&gt;</t>
-  </si>
-  <si>
-    <t>&lt;b&gt;&lt;span style="color:#8304BA"&gt; Quiz 9 due&lt;/span&gt;&lt;/b&gt;</t>
-  </si>
-  <si>
-    <t>&lt;b&gt;&lt;span style="color:#8304BA"&gt; Quiz 10 due&lt;/span&gt;&lt;/b&gt;</t>
-  </si>
-  <si>
     <t>Weekly Module</t>
   </si>
   <si>
@@ -309,9 +279,6 @@
     <t>Su: April 6, 2025</t>
   </si>
   <si>
-    <t>Su: April 14, 2025</t>
-  </si>
-  <si>
     <t>Su: April 20, 2025</t>
   </si>
   <si>
@@ -330,9 +297,6 @@
     <t>&lt;b&gt;&lt;span style="color:#D3CA09"&gt; Jennifer's Office Hours (7-9 pm, Kanbar 200)&lt;/span&gt;&lt;/b&gt;</t>
   </si>
   <si>
-    <t>&lt;b&gt;&lt;span style="color:#D3CA09"&gt; Jennifer: Midterm Review (7-9 pm, Kanbar 200)&lt;/span&gt;&lt;/b&gt;</t>
-  </si>
-  <si>
     <t>W: March 5, 2025</t>
   </si>
   <si>
@@ -343,6 +307,54 @@
   </si>
   <si>
     <t>&lt;b&gt;&lt;span style="color:#2bda19"&gt; Project: Group Contract due&lt;/span&gt;&lt;/b&gt;</t>
+  </si>
+  <si>
+    <t>Su:March 2, 2025</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;&lt;span style="color:#8304BA"&gt; Week 1 Quiz due&lt;/span&gt;&lt;/b&gt;</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;&lt;span style="color:#8304BA"&gt; Week 2 Quiz due &lt;/span&gt;&lt;/b&gt;</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;&lt;span style="color:#8304BA"&gt; Week 3 Quiz due&lt;/span&gt;&lt;/b&gt;</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;&lt;span style="color:#8304BA"&gt; Week 4 Quiz due&lt;/span&gt;&lt;/b&gt;</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;&lt;span style="color:#8304BA"&gt; Week 5 Quiz due&lt;/span&gt;&lt;/b&gt;</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;&lt;span style="color:#8304BA"&gt; Week 6 Quiz due&lt;/span&gt;&lt;/b&gt;</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;&lt;span style="color:#8304BA"&gt; Week 10 Quiz due&lt;/span&gt;&lt;/b&gt;</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;&lt;span style="color:#8304BA"&gt; Week 11 Quiz due&lt;/span&gt;&lt;/b&gt;</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;&lt;span style="color:#8304BA"&gt; Week 12 Quiz due&lt;/span&gt;&lt;/b&gt;</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;&lt;span style="color:#8304BA"&gt; Week 13 Quiz due&lt;/span&gt;&lt;/b&gt;</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;&lt;span style="color:#8304BA"&gt; Week 14 Quiz due&lt;/span&gt;&lt;/b&gt;</t>
+  </si>
+  <si>
+    <t>M: April 26, 2025</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;&lt;span style="color:#D3CA09"&gt; Jennifer's Office Hours (12-2 pm, Kanbar 200)&lt;/span&gt;&lt;/b&gt;</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;&lt;span style="color:#D3CA09"&gt; Jennifer: Midterm Review (4.30-6.30 pm, Kanbar 200)&lt;/span&gt;&lt;/b&gt;</t>
+  </si>
+  <si>
+    <t>Su: April 13, 2025</t>
   </si>
 </sst>
 </file>
@@ -761,10 +773,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:XFA52"/>
+  <dimension ref="A1:XFA53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="119" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="119" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -783,7 +795,7 @@
         <v>7</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:16381" ht="18">
@@ -794,7 +806,7 @@
         <v>8</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:16381" ht="18">
@@ -813,10 +825,10 @@
         <v>1</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>43</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:16381" s="1" customFormat="1" ht="18">
@@ -827,7 +839,7 @@
         <v>10</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="D5"/>
       <c r="E5"/>
@@ -9028,7 +9040,7 @@
         <v>11</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:16381" ht="18">
@@ -9036,10 +9048,10 @@
         <v>2</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>45</v>
+        <v>91</v>
       </c>
     </row>
     <row r="8" spans="1:16381" ht="34">
@@ -9047,10 +9059,10 @@
         <v>2</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9" spans="1:16381" ht="18">
@@ -9061,7 +9073,7 @@
         <v>12</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:16381" ht="16" customHeight="1">
@@ -9072,7 +9084,7 @@
         <v>13</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:16381" ht="18">
@@ -9083,7 +9095,7 @@
         <v>14</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="D11" s="1"/>
     </row>
@@ -9092,10 +9104,10 @@
         <v>3</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>46</v>
+        <v>92</v>
       </c>
     </row>
     <row r="13" spans="1:16381" ht="34">
@@ -9106,7 +9118,7 @@
         <v>15</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
     </row>
     <row r="14" spans="1:16381" ht="18">
@@ -9114,10 +9126,10 @@
         <v>3</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
     </row>
     <row r="15" spans="1:16381" ht="18">
@@ -9128,7 +9140,7 @@
         <v>16</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:16381" ht="18">
@@ -9136,10 +9148,10 @@
         <v>4</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>47</v>
+        <v>93</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="34">
@@ -9147,10 +9159,10 @@
         <v>4</v>
       </c>
       <c r="B17" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C17" s="10" t="s">
         <v>84</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="16" customHeight="1">
@@ -9161,7 +9173,7 @@
         <v>17</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="17" customHeight="1">
@@ -9172,7 +9184,7 @@
         <v>18</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="18">
@@ -9180,10 +9192,10 @@
         <v>5</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>51</v>
+        <v>94</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="18">
@@ -9191,10 +9203,10 @@
         <v>6</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="18">
@@ -9205,7 +9217,7 @@
         <v>19</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="16" customHeight="1">
@@ -9216,52 +9228,52 @@
         <v>20</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="18">
       <c r="A24">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="D24" s="1"/>
+        <v>89</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>95</v>
+      </c>
     </row>
-    <row r="25" spans="1:4" ht="34">
+    <row r="25" spans="1:4" ht="18">
       <c r="A25">
         <v>7</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="C25" s="10" t="s">
-        <v>96</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D25" s="1"/>
     </row>
-    <row r="26" spans="1:4" ht="15" customHeight="1">
+    <row r="26" spans="1:4" ht="34">
       <c r="A26">
         <v>7</v>
       </c>
       <c r="B26" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="15" customHeight="1">
+      <c r="A27">
+        <v>7</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C26" s="7" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="18">
-      <c r="A27">
-        <v>8</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>49</v>
+      <c r="C27" s="7" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="18">
@@ -9269,21 +9281,21 @@
         <v>8</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="18">
       <c r="A29">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="18">
@@ -9291,100 +9303,100 @@
         <v>9</v>
       </c>
       <c r="B30" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="18">
+      <c r="A31">
+        <v>9</v>
+      </c>
+      <c r="B31" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C30" s="4" t="s">
-        <v>49</v>
+      <c r="C31" s="4" t="s">
+        <v>45</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="20" customHeight="1">
-      <c r="A31">
-        <v>10</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D31" s="1"/>
-    </row>
-    <row r="32" spans="1:4" ht="18">
+    <row r="32" spans="1:4" ht="20" customHeight="1">
       <c r="A32">
         <v>10</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C32" s="8" t="s">
-        <v>71</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D32" s="1"/>
     </row>
     <row r="33" spans="1:4" ht="18">
       <c r="A33">
         <v>10</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="C33" s="6" t="s">
-        <v>52</v>
+        <v>28</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="18">
       <c r="A34">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C34" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="D34" s="8"/>
+        <v>77</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="35" spans="1:4" ht="18">
       <c r="A35">
         <v>11</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>72</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="D35" s="8"/>
     </row>
     <row r="36" spans="1:4" ht="18">
       <c r="A36">
         <v>11</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="C36" s="6" t="s">
-        <v>53</v>
+        <v>30</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>62</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="34">
+    <row r="37" spans="1:4" ht="18">
       <c r="A37">
         <v>11</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="C37" s="10" t="s">
-        <v>95</v>
+        <v>78</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>97</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="18">
+    <row r="38" spans="1:4" ht="34">
       <c r="A38">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C38" s="11" t="s">
         <v>78</v>
+      </c>
+      <c r="C38" s="10" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="18">
@@ -9392,43 +9404,43 @@
         <v>12</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>64</v>
+        <v>31</v>
+      </c>
+      <c r="C39" s="11" t="s">
+        <v>68</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="17" customHeight="1">
+    <row r="40" spans="1:4" ht="18">
       <c r="A40">
         <v>12</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C40" s="8" t="s">
-        <v>73</v>
+        <v>32</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>54</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="18">
+    <row r="41" spans="1:4" ht="17" customHeight="1">
       <c r="A41">
         <v>12</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="C41" s="6" t="s">
-        <v>54</v>
+        <v>33</v>
+      </c>
+      <c r="C41" s="8" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="18">
       <c r="A42">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>65</v>
+        <v>104</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="18">
@@ -9436,10 +9448,10 @@
         <v>13</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>74</v>
+        <v>55</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="18">
@@ -9447,21 +9459,21 @@
         <v>13</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="C44" s="6" t="s">
-        <v>55</v>
+        <v>35</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="18">
       <c r="A45">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C45" s="8" t="s">
-        <v>66</v>
+        <v>79</v>
+      </c>
+      <c r="C45" s="6" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="18">
@@ -9469,10 +9481,10 @@
         <v>14</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>75</v>
+        <v>36</v>
+      </c>
+      <c r="C46" s="8" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="18">
@@ -9480,32 +9492,32 @@
         <v>14</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="C47" s="6" t="s">
-        <v>56</v>
+        <v>37</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>65</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="34">
+    <row r="48" spans="1:4" ht="18">
       <c r="A48">
+        <v>14</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C48" s="6" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="34">
+      <c r="A49">
         <v>11</v>
       </c>
-      <c r="B48" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="C48" s="10" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" ht="18">
-      <c r="A49">
-        <v>15</v>
-      </c>
       <c r="B49" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C49" s="12" t="s">
-        <v>79</v>
+        <v>101</v>
+      </c>
+      <c r="C49" s="10" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="18">
@@ -9513,34 +9525,45 @@
         <v>15</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C50" s="13" t="s">
-        <v>60</v>
+        <v>38</v>
+      </c>
+      <c r="C50" s="12" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="18">
       <c r="A51">
+        <v>15</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C51" s="13" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="18">
+      <c r="A52">
         <v>16</v>
       </c>
-      <c r="B51" s="2" t="s">
+      <c r="B52" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C51" s="1" t="s">
-        <v>80</v>
+      <c r="C52" s="1" t="s">
+        <v>70</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="17" customHeight="1">
-      <c r="A52">
+    <row r="53" spans="1:4" ht="17" customHeight="1">
+      <c r="A53">
         <v>17</v>
       </c>
-      <c r="B52" s="2" t="s">
+      <c r="B53" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C52" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="D52" s="1"/>
+      <c r="C53" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="D53" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>